<commit_message>
Added two new sheets to python questions
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions.xlsx
+++ b/PythonPals/python_questions.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheam\PycharmProjects\pythonPals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Sheamus\School\Senior\Python\PythonPals\PythonPals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6014502A-1001-45EC-83AD-7EBFAFDF17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A415230-A0BA-4720-BDF5-0BED9571BC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
+    <workbookView xWindow="-8988" yWindow="5796" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Default" sheetId="1" r:id="rId1"/>
+    <sheet name="Capitals" sheetId="2" r:id="rId2"/>
+    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="311">
   <si>
     <t>Number</t>
   </si>
@@ -533,12 +535,625 @@
   <si>
     <t>D. 13</t>
   </si>
+  <si>
+    <t>What is the capital of France?</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>What is the capital of the United Kingdom?</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Tunis</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>What is the capital of Switzerland?</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>What is the capital of Austria?</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Tehran</t>
+  </si>
+  <si>
+    <t>What is the capital of Sweden?</t>
+  </si>
+  <si>
+    <t>Helsinki</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>What is the capital of China?</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh City</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>What is the capital of Mongolia?</t>
+  </si>
+  <si>
+    <t>Ulaanbaatar</t>
+  </si>
+  <si>
+    <t>Kathmundu</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Kashmir</t>
+  </si>
+  <si>
+    <t>What is the capital of Indonesia?</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>What is the capital of India?</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Islamabad</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>What is the capital of Turkmenistan?</t>
+  </si>
+  <si>
+    <t>Baghdad</t>
+  </si>
+  <si>
+    <t>Ashgabat</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>The Americas</t>
+  </si>
+  <si>
+    <t>What is the capital of Mexico?</t>
+  </si>
+  <si>
+    <t>Mexico City</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Tijuana</t>
+  </si>
+  <si>
+    <t>What is the capital of Uruguay?</t>
+  </si>
+  <si>
+    <t>Montevideo</t>
+  </si>
+  <si>
+    <t>La Paz</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Caracas</t>
+  </si>
+  <si>
+    <t>What is the capital of Brazil?</t>
+  </si>
+  <si>
+    <t>Sao Paulo</t>
+  </si>
+  <si>
+    <t>Manaus</t>
+  </si>
+  <si>
+    <t>What is the capital of the United States of America?</t>
+  </si>
+  <si>
+    <t>Washington D.C.</t>
+  </si>
+  <si>
+    <t>New York City</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>What is the capital of Cuba?</t>
+  </si>
+  <si>
+    <t>Havana</t>
+  </si>
+  <si>
+    <t>Tahiti</t>
+  </si>
+  <si>
+    <t>Santo Domingo</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>What is the capital of Australia?</t>
+  </si>
+  <si>
+    <t>Canberra</t>
+  </si>
+  <si>
+    <t>Perth</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>What is the capital of South Africa?</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Timbuktu</t>
+  </si>
+  <si>
+    <t>What is the capital of New Zealand?</t>
+  </si>
+  <si>
+    <t>Christchurch</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Queenstown</t>
+  </si>
+  <si>
+    <t>Waipara</t>
+  </si>
+  <si>
+    <t>What is the capital of Ethiopia?</t>
+  </si>
+  <si>
+    <t>Addis Abbaba</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>Mogadishu</t>
+  </si>
+  <si>
+    <t>Tel Aviv</t>
+  </si>
+  <si>
+    <t>What is the capital of Palau?</t>
+  </si>
+  <si>
+    <t>Ngelrulmud</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Which of these events happened first?</t>
+  </si>
+  <si>
+    <t>Earliest</t>
+  </si>
+  <si>
+    <t>WWI</t>
+  </si>
+  <si>
+    <t>Sinking of the Titanic</t>
+  </si>
+  <si>
+    <t>Great Depression</t>
+  </si>
+  <si>
+    <t>First Man on the Moon</t>
+  </si>
+  <si>
+    <t>Reichstag Fire</t>
+  </si>
+  <si>
+    <t>Germany invades Poland</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Benito Mussolini becomes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Il Duce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of Italy</t>
+    </r>
+  </si>
+  <si>
+    <t>Eruption at Pompeii</t>
+  </si>
+  <si>
+    <t>Julius Ceaser is killed</t>
+  </si>
+  <si>
+    <t>Death of Alexander the Great</t>
+  </si>
+  <si>
+    <t>Burning of the Library of Alexandria</t>
+  </si>
+  <si>
+    <t>Nuremberg Trials</t>
+  </si>
+  <si>
+    <t>Hindenberg Disaster</t>
+  </si>
+  <si>
+    <t>Woodrow Wilson becomes US President</t>
+  </si>
+  <si>
+    <t>Napoleon Bonaparte dies</t>
+  </si>
+  <si>
+    <t>Japan invades Manchuria</t>
+  </si>
+  <si>
+    <t>Mao Zedong is born</t>
+  </si>
+  <si>
+    <t>Hong Kong is released from British rule</t>
+  </si>
+  <si>
+    <t>First confirmed summit of Mount Everest</t>
+  </si>
+  <si>
+    <t>Latest</t>
+  </si>
+  <si>
+    <t>Which of these events happened last?</t>
+  </si>
+  <si>
+    <t>Black Plague reaches Europe</t>
+  </si>
+  <si>
+    <t>Charlemagne dies</t>
+  </si>
+  <si>
+    <t>Start of the First Crusade</t>
+  </si>
+  <si>
+    <t>Martin Luther nails his 95 Theses</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Machiavelli writes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Prince</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chaucer publishes his </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Canterbury Tales</t>
+    </r>
+  </si>
+  <si>
+    <t>Jane Austen is born</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Jane Eyre </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is published</t>
+    </r>
+  </si>
+  <si>
+    <t>Marie Curie discovers Uranium</t>
+  </si>
+  <si>
+    <t>First cells observed under a microscope</t>
+  </si>
+  <si>
+    <t>Einstein publishes his General Theory of Relativity</t>
+  </si>
+  <si>
+    <t>Radio is invented</t>
+  </si>
+  <si>
+    <t>Newton describes his laws of motion</t>
+  </si>
+  <si>
+    <t>End of the Seven Year's War</t>
+  </si>
+  <si>
+    <t>Napoleon Bonaparte is born</t>
+  </si>
+  <si>
+    <t>Revolutions of 1848</t>
+  </si>
+  <si>
+    <t>Korean War ends</t>
+  </si>
+  <si>
+    <t>Start of First Gulf War</t>
+  </si>
+  <si>
+    <t>US withdraws from Vietnam</t>
+  </si>
+  <si>
+    <t>US invasion of Iraq</t>
+  </si>
+  <si>
+    <t>Which of these events occurred in the nineteenth century?</t>
+  </si>
+  <si>
+    <t>US Civil War</t>
+  </si>
+  <si>
+    <t>US Constitution is ratified</t>
+  </si>
+  <si>
+    <t>Alaska becomes a US state</t>
+  </si>
+  <si>
+    <t>Century</t>
+  </si>
+  <si>
+    <t>Which of these events occurred in the seventeenth century?</t>
+  </si>
+  <si>
+    <t>Queen Elizabeth I dies</t>
+  </si>
+  <si>
+    <t>Seven Year's War</t>
+  </si>
+  <si>
+    <t>Signing of the Declaration of Independence</t>
+  </si>
+  <si>
+    <t>Columbus discovers America</t>
+  </si>
+  <si>
+    <t>Magellan's crew circumnavigates the globe</t>
+  </si>
+  <si>
+    <t>US makes the Louisiana Purchase from France</t>
+  </si>
+  <si>
+    <t>Assassination of Archduke Franz Ferdinand</t>
+  </si>
+  <si>
+    <t>Which of these events occurred in the twentieth century?</t>
+  </si>
+  <si>
+    <t>Ronald Reagan is inaugurated as U.S. President</t>
+  </si>
+  <si>
+    <t>South Sudan becomes an independent nation</t>
+  </si>
+  <si>
+    <t>Facebook is founded</t>
+  </si>
+  <si>
+    <t>Teddy Roosevelt is born</t>
+  </si>
+  <si>
+    <t>Which of these events occurred in the twenty-first century?</t>
+  </si>
+  <si>
+    <t>Bill Clinton is elected U.S. president</t>
+  </si>
+  <si>
+    <t>Completion of the Human Genome Project</t>
+  </si>
+  <si>
+    <t>First sheep cloned</t>
+  </si>
+  <si>
+    <t>First Gulf War</t>
+  </si>
+  <si>
+    <t>Which of these people was born first?</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Harry S. Truman</t>
+  </si>
+  <si>
+    <t>Mao Zedong</t>
+  </si>
+  <si>
+    <t>John F. Kennedy</t>
+  </si>
+  <si>
+    <t>Josef Stalin</t>
+  </si>
+  <si>
+    <t>Barack Obama</t>
+  </si>
+  <si>
+    <t>Joseph Biden</t>
+  </si>
+  <si>
+    <t>Bill Clinton</t>
+  </si>
+  <si>
+    <t>Nelson Mandela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin Luther King Jr. </t>
+  </si>
+  <si>
+    <t>Hillary Clinton</t>
+  </si>
+  <si>
+    <t>Malcolm X</t>
+  </si>
+  <si>
+    <t>Booker T. Washington</t>
+  </si>
+  <si>
+    <t>Helmut Kohl</t>
+  </si>
+  <si>
+    <t>Angela Merkel</t>
+  </si>
+  <si>
+    <t>Otto Von Bismarck</t>
+  </si>
+  <si>
+    <t>Adolf Hitler</t>
+  </si>
+  <si>
+    <t>Emmanuel Macron</t>
+  </si>
+  <si>
+    <t>David Cameron</t>
+  </si>
+  <si>
+    <t>Boris Johnson</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +1164,14 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,7 +1197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -583,6 +1206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D33FE3-95A4-4979-84F6-48E46D9AB26E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="47" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="B13" zoomScale="47" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1528,4 +2152,1064 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E03268-21A2-4836-85AC-DD011DFA9BC1}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" t="s">
+        <v>204</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" t="s">
+        <v>209</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" t="s">
+        <v>218</v>
+      </c>
+      <c r="H20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E31CADC-C786-460E-9910-31504D11CF7C}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" customWidth="1"/>
+    <col min="7" max="7" width="50.21875" customWidth="1"/>
+    <col min="8" max="8" width="41.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G4" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>255</v>
+      </c>
+      <c r="F9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G9" t="s">
+        <v>257</v>
+      </c>
+      <c r="H9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G11" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" t="s">
+        <v>227</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>276</v>
+      </c>
+      <c r="F14" t="s">
+        <v>277</v>
+      </c>
+      <c r="G14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" t="s">
+        <v>282</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" t="s">
+        <v>287</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="H16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F17" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H17" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F18" t="s">
+        <v>297</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H18" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B19" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F19" t="s">
+        <v>300</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H19" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F20" t="s">
+        <v>305</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" t="s">
+        <v>305</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed excel logic questions format
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions.xlsx
+++ b/PythonPals/python_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheam\PycharmProjects\pythonPals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/abd7a485bb1aa73f/UF/Fall2020/Python/Project/PythonPals/PythonPals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6014502A-1001-45EC-83AD-7EBFAFDF17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6014502A-1001-45EC-83AD-7EBFAFDF17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FBB5D87-0FF9-44F3-A218-1E7921C6F7A4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
+    <workbookView xWindow="-28920" yWindow="-1365" windowWidth="29040" windowHeight="15840" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,33 +124,16 @@
 D. 4 </t>
   </si>
   <si>
-    <t>What is the output of the following code? list = [ 'one', 'two']
-for i in list:
-	list.append(i.upper())
-	print(list)</t>
-  </si>
-  <si>
     <t>A. ['one', 'two']
 B. ['one, 'two', 'one', 'two']
 C. ['one', 'two', 'one']
 D. No Output</t>
   </si>
   <si>
-    <t>What is the output of the following code? dictionary = {1: 'first', 2: 'second', 3: 'third', 4: 'fourth'}
-del dictionary[1]
-dictionary[1] = '42'
-del dictionary[2]
-print len(dictionary)</t>
-  </si>
-  <si>
     <t>A. 1
 B. 2
 C. 3 
 D. 4</t>
-  </si>
-  <si>
-    <t>What is the output of the following code? names = ['John', 'Paul', 'George', 'Ringo']
-print names[1][-2]</t>
   </si>
   <si>
     <t>A. h
@@ -532,6 +515,26 @@
   </si>
   <si>
     <t>D. 13</t>
+  </si>
+  <si>
+    <t>What is the output of the following code? 
+        names = ['John', 'Paul', 'George', 'Ringo']
+        print(names[1][-2])</t>
+  </si>
+  <si>
+    <t>What is the output of the following code? 
+dictionary = {1: 'first', 2: 'second', 3: 'third', 4: 'fourth'}
+del dictionary[1]
+dictionary[1] = '42'
+del dictionary[2]
+print len(dictionary)</t>
+  </si>
+  <si>
+    <t>What is the output of the following code? 
+list = [ 'one', 'two']
+for i in list:
+	list.append(i.upper())
+	print(list)</t>
   </si>
 </sst>
 </file>
@@ -899,23 +902,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D33FE3-95A4-4979-84F6-48E46D9AB26E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="47" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="5.21875" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="33.44140625" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="63.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,48 +935,48 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -981,28 +984,28 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1010,28 +1013,28 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
         <v>67</v>
       </c>
-      <c r="H4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1039,28 +1042,28 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1068,28 +1071,28 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>69</v>
       </c>
-      <c r="I6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1097,28 +1100,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
         <v>76</v>
       </c>
-      <c r="G7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1126,28 +1129,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" t="s">
         <v>80</v>
       </c>
-      <c r="G8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1155,28 +1158,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" t="s">
         <v>84</v>
       </c>
-      <c r="G9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1184,28 +1187,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" t="s">
         <v>89</v>
       </c>
-      <c r="G10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1213,28 +1216,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>20</v>
@@ -1251,19 +1254,19 @@
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" t="s">
         <v>96</v>
       </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>22</v>
@@ -1280,106 +1283,106 @@
         <v>15</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
       <c r="F14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
         <v>104</v>
       </c>
-      <c r="G14" t="s">
-        <v>105</v>
-      </c>
-      <c r="H14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G16" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="I16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1387,28 +1390,28 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1416,112 +1419,112 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="I18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed multi line questions
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions.xlsx
+++ b/PythonPals/python_questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/abd7a485bb1aa73f/UF/Fall2020/Python/Project/PythonPals/PythonPals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Sheamus\School\Senior\Python\PythonPals\PythonPals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6014502A-1001-45EC-83AD-7EBFAFDF17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FBB5D87-0FF9-44F3-A218-1E7921C6F7A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9752A85C-F3E5-4126-B1BE-9BC6101909FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1365" windowWidth="29040" windowHeight="15840" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="129">
   <si>
     <t>Number</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Correct Answer</t>
   </si>
   <si>
-    <t>Which of these code snippets will compile in Python?</t>
-  </si>
-  <si>
     <t>Which of these is not a reserved Python keyword?</t>
   </si>
   <si>
@@ -91,11 +88,6 @@
   </si>
   <si>
     <t>For which of these concepts does Python have built in support?</t>
-  </si>
-  <si>
-    <t>What is the output of the following code? 
-arbitraryTuple = (2, 5)
-print 2 * arbitraryTuple</t>
   </si>
   <si>
     <t>A. (2, 5, 2, 5) 
@@ -104,49 +96,7 @@
 D. (2, 2, 5, 5)</t>
   </si>
   <si>
-    <t>What is the output of the following code? 
-a = True
-b = True
-c = False
-if not a or not b:
-	print 1
-elif not a or b and c:
-	print 2
-elif not a or not b or b and a:
-	print 3
-else:
-	print 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. 1
-B. 2
-C. 3 
-D. 4 </t>
-  </si>
-  <si>
-    <t>A. ['one', 'two']
-B. ['one, 'two', 'one', 'two']
-C. ['one', 'two', 'one']
-D. No Output</t>
-  </si>
-  <si>
-    <t>A. 1
-B. 2
-C. 3 
-D. 4</t>
-  </si>
-  <si>
-    <t>A. h
-B. u 
-C. o
-D. a</t>
-  </si>
-  <si>
     <t>Number Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How would you declare a class named Foo with a variable for 'name' set to "Espresso"? 
-</t>
   </si>
   <si>
     <t>A. 'True'
@@ -173,18 +123,6 @@
 D. 11111000</t>
   </si>
   <si>
-    <t xml:space="preserve">                A. class Foo:
-		def name = "Espresso"
-	B. class Foo: 
-		def __init__(self):
-			self.name = "Espresso"
-	C. def class Foo: 
-		name = "Espresso"
-	D. class Foo:
-		__init__(name)
-			name = "Espresso"</t>
-  </si>
-  <si>
     <t>Syntax</t>
   </si>
   <si>
@@ -269,50 +207,6 @@
     <t>Choice 4</t>
   </si>
   <si>
-    <t>B. class Foo: 
-		def __init__(self):
-			self.name = "Espresso"</t>
-  </si>
-  <si>
-    <t>A. class Foo:
-		def name = "Espresso"</t>
-  </si>
-  <si>
-    <t>C. def class Foo: 
-		name = "Espresso"</t>
-  </si>
-  <si>
-    <t>D. class Foo:
-		__init__(name)
-			name = "Espresso"</t>
-  </si>
-  <si>
-    <t>A. if 4 == 3
-	print(True)</t>
-  </si>
-  <si>
-    <t>A. if 4 == 3
-	print(True)
-B. if 4 == 3:
-     print(True)
-C. if 4 == 3:  
-	print(True)
-D. if 4 == 3
-     print(true)</t>
-  </si>
-  <si>
-    <t>B. if 4 == 3:
-     print(True)</t>
-  </si>
-  <si>
-    <t>C. if 4 == 3:  
-	print(True)</t>
-  </si>
-  <si>
-    <t>D. if 4 == 3
-     print(true)</t>
-  </si>
-  <si>
     <t>A. 'True'</t>
   </si>
   <si>
@@ -421,9 +315,6 @@
     <t>D. (2, 2, 5, 5)</t>
   </si>
   <si>
-    <t>D. 4</t>
-  </si>
-  <si>
     <t>A. 1</t>
   </si>
   <si>
@@ -433,33 +324,9 @@
     <t>C. 3</t>
   </si>
   <si>
-    <t>A. ['one', 'two']</t>
-  </si>
-  <si>
-    <t>B. ['one, 'two', 'one', 'two']</t>
-  </si>
-  <si>
-    <t>C. ['one', 'two', 'one']</t>
-  </si>
-  <si>
-    <t>D. No Output</t>
-  </si>
-  <si>
-    <t>A. h</t>
-  </si>
-  <si>
     <t>A. a1</t>
   </si>
   <si>
-    <t>B. u</t>
-  </si>
-  <si>
-    <t>C. o</t>
-  </si>
-  <si>
-    <t>D. a</t>
-  </si>
-  <si>
     <t>D. fe</t>
   </si>
   <si>
@@ -517,24 +384,85 @@
     <t>D. 13</t>
   </si>
   <si>
-    <t>What is the output of the following code? 
-        names = ['John', 'Paul', 'George', 'Ringo']
-        print(names[1][-2])</t>
-  </si>
-  <si>
-    <t>What is the output of the following code? 
-dictionary = {1: 'first', 2: 'second', 3: 'third', 4: 'fourth'}
-del dictionary[1]
-dictionary[1] = '42'
-del dictionary[2]
-print len(dictionary)</t>
-  </si>
-  <si>
-    <t>What is the output of the following code? 
-list = [ 'one', 'two']
-for i in list:
-	list.append(i.upper())
-	print(list)</t>
+    <t>How is a class declared in Python?</t>
+  </si>
+  <si>
+    <t>A. def class Foo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. class Foo: </t>
+  </si>
+  <si>
+    <t>C. Foo class:</t>
+  </si>
+  <si>
+    <t>D. class def Foo:</t>
+  </si>
+  <si>
+    <t>What is the value of t after the line: t = 2 * (2,5) ?</t>
+  </si>
+  <si>
+    <t>How would you declare a derived class in Python?</t>
+  </si>
+  <si>
+    <t>A. def Bar: Foo:</t>
+  </si>
+  <si>
+    <t>B. def Bar is Foo:</t>
+  </si>
+  <si>
+    <t>D. def</t>
+  </si>
+  <si>
+    <t>C. def class Bar(Foo):</t>
+  </si>
+  <si>
+    <t>D. def Bar(Foo):</t>
+  </si>
+  <si>
+    <t>Which command is used to exit a while loop?</t>
+  </si>
+  <si>
+    <t>A. continue</t>
+  </si>
+  <si>
+    <t>B. out</t>
+  </si>
+  <si>
+    <t>C. for</t>
+  </si>
+  <si>
+    <t>D. break</t>
+  </si>
+  <si>
+    <t>What is the value of 15 % 2?</t>
+  </si>
+  <si>
+    <t>A. 5</t>
+  </si>
+  <si>
+    <t>D. 1</t>
+  </si>
+  <si>
+    <t>What is the value of 18 % 3?</t>
+  </si>
+  <si>
+    <t>C. 0</t>
+  </si>
+  <si>
+    <t>D. 3</t>
+  </si>
+  <si>
+    <t>Which of the following commands can be used to bring in code from other files?</t>
+  </si>
+  <si>
+    <t>A. find</t>
+  </si>
+  <si>
+    <t>B. import</t>
+  </si>
+  <si>
+    <t>C. include</t>
   </si>
 </sst>
 </file>
@@ -902,23 +830,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D33FE3-95A4-4979-84F6-48E46D9AB26E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="86" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -935,596 +863,584 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="G13" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="I16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="I20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="I21" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited python excel file to fit q's on screen
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions.xlsx
+++ b/PythonPals/python_questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Sheamus\School\Senior\Python\PythonPals\PythonPals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/abd7a485bb1aa73f/UF/Fall2020/Python/Project/PythonPals/PythonPals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB195BA-AD9C-430A-96A5-2E5BF4208695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{DE46B356-965D-4870-9C83-F8518D896B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DEE8B906-3FBA-4595-BC00-D223B1005E96}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>What characterizes a high-level programming language?</t>
   </si>
   <si>
-    <t>What is the name of the output of a compiler after it translates the program?</t>
-  </si>
-  <si>
     <t>What is the hexadecimal representation of the binary 100001?</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>For which of these concepts does Python have built in support?</t>
   </si>
   <si>
     <t>A. (2, 5, 2, 5) 
@@ -453,9 +447,6 @@
     <t>D. 3</t>
   </si>
   <si>
-    <t>Which of the following commands can be used to bring in code from other files?</t>
-  </si>
-  <si>
     <t>A. find</t>
   </si>
   <si>
@@ -463,6 +454,18 @@
   </si>
   <si>
     <t>C. include</t>
+  </si>
+  <si>
+    <t>For which of these concepts does Python
+have built in support?</t>
+  </si>
+  <si>
+    <t>What is the name of the output of a compiler
+after it translates the program?</t>
+  </si>
+  <si>
+    <t>Which of the following commands can be used to
+ bring in code from other files?</t>
   </si>
 </sst>
 </file>
@@ -830,23 +833,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D33FE3-95A4-4979-84F6-48E46D9AB26E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="33.44140625" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="63.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -863,73 +866,73 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -937,28 +940,28 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -966,57 +969,57 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1024,28 +1027,28 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
         <v>55</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1053,28 +1056,28 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
         <v>59</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>60</v>
       </c>
-      <c r="H8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1082,28 +1085,28 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>64</v>
       </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1111,336 +1114,336 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>69</v>
       </c>
-      <c r="H10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
+      <c r="B11" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" t="s">
         <v>72</v>
       </c>
-      <c r="G11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" t="s">
-        <v>74</v>
-      </c>
       <c r="I11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
         <v>115</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>116</v>
       </c>
-      <c r="H14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="I17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>